<commit_message>
new dataset with corrected column names
</commit_message>
<xml_diff>
--- a/combined_input_output_summary.xlsx
+++ b/combined_input_output_summary.xlsx
@@ -481,20 +481,30 @@
           <t>Min</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>27.2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>9</v>
-      </c>
-      <c r="E2" t="n">
-        <v>16</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.203977338</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.3154388666152954</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>51.80</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>3.20</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.0860</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.1309</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -508,20 +518,30 @@
           <t>Mean</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>42.4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>220</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.836163619845</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.8344200253486633</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>11.40</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4.20</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>74.20</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.7505</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.7520</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -535,20 +555,30 @@
           <t>Max</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>47.29999999999999</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E4" t="n">
-        <v>970</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.9477275759999999</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.9459196925163269</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>53.60</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8.20</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>60.50</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.9420</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.9262</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -562,20 +592,30 @@
           <t>Min</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>27.2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>9</v>
-      </c>
-      <c r="E5" t="n">
-        <v>16</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.8551582098007202</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>51.80</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3.20</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.2630</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.4089</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -589,20 +629,30 @@
           <t>Mean</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>15.3</v>
-      </c>
-      <c r="D6" t="n">
-        <v>5.2</v>
-      </c>
-      <c r="E6" t="n">
-        <v>605</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1.8372125</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.831094861030579</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>11.50</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>4.00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>53.20</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1.6776</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1.6784</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -616,20 +666,30 @@
           <t>Max</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>43.2</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E7" t="n">
-        <v>928</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1.955641388893127</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>54.70</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>9.50</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>41.40</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2.2000</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2.1423</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -643,20 +703,30 @@
           <t>Min</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>27.2</v>
-      </c>
-      <c r="D8" t="n">
-        <v>9</v>
-      </c>
-      <c r="E8" t="n">
-        <v>16</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1.932454943656921</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>51.80</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>3.20</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0.6520</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.9920</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -670,20 +740,30 @@
           <t>Mean</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>15.6</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E9" t="n">
-        <v>164</v>
-      </c>
-      <c r="F9" t="n">
-        <v>3.567625</v>
-      </c>
-      <c r="G9" t="n">
-        <v>3.573834419250488</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>54.80</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>4.40</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>14.90</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>3.1613</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>3.1456</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -697,20 +777,30 @@
           <t>Max</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>47.29999999999999</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E10" t="n">
-        <v>970</v>
-      </c>
-      <c r="F10" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="G10" t="n">
-        <v>3.76421594619751</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>34.10</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>9.90</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>63.30</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>4.1000</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>4.0157</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>